<commit_message>
Completed Python analysis of lab 6 (probably)
I analyzed the causes of wildfires
</commit_message>
<xml_diff>
--- a/Lab 6/Fire Perimeter/Causes description.xlsx
+++ b/Lab 6/Fire Perimeter/Causes description.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LMAOXD\Documents\UCI undergrad\4th year (last year)\Winter 2021\ESS 162 - all about California\Lab 6\Fire Perimeter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2420EDD2-C145-4138-8B02-EA3CD00A0840}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A03BF285-9F8F-4B86-A4C0-7BAFF454E2C1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{56DE770A-8C51-4595-9EDF-22008E5C65BD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Cause Code</t>
   </si>
@@ -100,6 +100,18 @@
   </si>
   <si>
     <t>Data source: https://frap.fire.ca.gov/frap-projects/fire-perimeters/</t>
+  </si>
+  <si>
+    <t>The last 3 categories are all from me from combining the original categories</t>
+  </si>
+  <si>
+    <t>Manmade</t>
+  </si>
+  <si>
+    <t>Natural</t>
+  </si>
+  <si>
+    <t>Miscellaneous/Unknown</t>
   </si>
 </sst>
 </file>
@@ -142,7 +154,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -165,16 +177,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -491,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1783EC9-D529-4A89-84FE-4A4DFCF9800C}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -520,6 +546,9 @@
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="3" spans="1:3" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -649,7 +678,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -657,12 +686,36 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>